<commit_message>
Added headerRow static parameter
</commit_message>
<xml_diff>
--- a/tests/FSharpx.TypeProviders.Excel.Tests/BookTest.xlsx
+++ b/tests/FSharpx.TypeProviders.Excel.Tests/BookTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="22995" windowHeight="15645" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="22995" windowHeight="15645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
   </sheets>
   <definedNames>
     <definedName name="ThisIsaRange">Sheet1!$E$19:$X$20</definedName>
-    <definedName name="toto">Sheet1!$C$8:$J$20</definedName>
   </definedNames>
   <calcPr calcId="114210"/>
 </workbook>
@@ -499,7 +498,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -766,7 +765,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>